<commit_message>
"fixing it up still no orhcestrator"
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine.Moore\Documents\UiPath\HUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724AE8E-CEE0-4D16-96A5-E923E8CC7B93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CCF22B-594E-430E-B56A-AC56F170E1DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="9600" windowHeight="4970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="3" r:id="rId1"/>
@@ -25,74 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
-  <si>
-    <t>The Incredibles 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Movie Name</t>
   </si>
   <si>
-    <t>Trailer Name</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Incredibles 2 Official Trailer</t>
-  </si>
-  <si>
-    <t>/watch?v=i5qOzqD9Rms&amp;t=3s</t>
-  </si>
-  <si>
-    <t>INCREDIBLES 2 Official Trailer #2 (2018) Disney Animated Superhero Movie HD</t>
-  </si>
-  <si>
-    <t>/watch?v=JwwY8gx_2LA</t>
-  </si>
-  <si>
-    <t>Incredibles 2 Official Teaser Trailer</t>
-  </si>
-  <si>
-    <t>/watch?v=ZJDMWVZta3M</t>
-  </si>
-  <si>
-    <t>Views</t>
-  </si>
-  <si>
-    <t>Likes</t>
-  </si>
-  <si>
-    <t>Dislikes</t>
-  </si>
-  <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>Published Date</t>
-  </si>
-  <si>
-    <t>56,896,468 views</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_x000D_
-   _x000D_
- </t>
-  </si>
-  <si>
-    <t>Published on Apr 13, 2018</t>
-  </si>
-  <si>
-    <t>2,068,703 views</t>
-  </si>
-  <si>
-    <t>Published on Feb 14, 2018</t>
-  </si>
-  <si>
-    <t>88,234,305 views</t>
-  </si>
-  <si>
-    <t>Published on Nov 18, 2017</t>
+    <t>It</t>
   </si>
 </sst>
 </file>
@@ -108,24 +46,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFE0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,15 +66,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BF02A3-3282-414E-ABDD-8E45600DA7E8}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,115 +369,44 @@
     <col min="5" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1">
-        <v>417981</v>
-      </c>
-      <c r="F2" s="1">
-        <v>20141</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1">
-        <v>25365</v>
-      </c>
-      <c r="F3" s="1">
-        <v>718</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1">
-        <v>522980</v>
-      </c>
-      <c r="F4" s="1">
-        <v>36006</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>

</xml_diff>

<commit_message>
"Reading in both files"
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine.Moore\Documents\UiPath\HUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CCF22B-594E-430E-B56A-AC56F170E1DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF10E897-89B0-44F8-9A05-9BD1416DB934}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="9600" windowHeight="4970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="3" r:id="rId1"/>
@@ -25,12 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Movie Name</t>
   </si>
   <si>
+    <t>Black Panther</t>
+  </si>
+  <si>
+    <t>Interstellar</t>
+  </si>
+  <si>
     <t>It</t>
+  </si>
+  <si>
+    <t>Star Wars: The Last Jedi</t>
+  </si>
+  <si>
+    <t>Ready Player One</t>
+  </si>
+  <si>
+    <t>Movie List 2</t>
+  </si>
+  <si>
+    <t>Incredibles 2</t>
+  </si>
+  <si>
+    <t>Avengers: Infinity War</t>
+  </si>
+  <si>
+    <t>The Lego Batman Movie</t>
+  </si>
+  <si>
+    <t>The Boss Baby</t>
+  </si>
+  <si>
+    <t>Inside Out</t>
   </si>
 </sst>
 </file>
@@ -354,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BF02A3-3282-414E-ABDD-8E45600DA7E8}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -384,32 +414,71 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first change to orchestrator
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine.Moore\Documents\UiPath\HUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388C3B51-BF20-4200-9E3F-E6F107DCB1C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1DB746-318F-4FBF-9FC5-AC88361802E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="9600" windowHeight="4970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="570" windowWidth="9600" windowHeight="4965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="3" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Movie Name</t>
   </si>
   <si>
-    <t>Interstellar</t>
-  </si>
-  <si>
     <t>It</t>
   </si>
   <si>
@@ -58,6 +55,174 @@
   </si>
   <si>
     <t>Black Panther</t>
+  </si>
+  <si>
+    <t>Trailer Name</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Marvel Studios' Black Panther - Official Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=xjDjIWPwcPU&amp;t=49s</t>
+  </si>
+  <si>
+    <t>Black Panther Teaser Trailer [HD]</t>
+  </si>
+  <si>
+    <t>/watch?v=dxWvtMOGAhw&amp;t=4s</t>
+  </si>
+  <si>
+    <t>Black Panther Official Trailer #1 (2018) Chadwick Boseman Marvel Movie HD</t>
+  </si>
+  <si>
+    <t>/watch?v=yLNLPECROMA&amp;t=3s</t>
+  </si>
+  <si>
+    <t>IT - Official Trailer 1</t>
+  </si>
+  <si>
+    <t>/watch?v=xKJmEC5ieOk&amp;t=6s</t>
+  </si>
+  <si>
+    <t>Last Christmas - Official Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=z9CEIcmWmtA</t>
+  </si>
+  <si>
+    <t>IT - Official Teaser Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=FnCdOQsX5kc&amp;t=3s</t>
+  </si>
+  <si>
+    <t>Star Wars: The Last Jedi Trailer (Official)</t>
+  </si>
+  <si>
+    <t>/watch?v=Q0CbN8sfihY</t>
+  </si>
+  <si>
+    <t>Star Wars: The Last Jedi Official Teaser</t>
+  </si>
+  <si>
+    <t>/watch?v=zB4I68XVPzQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STAR WARS: THE LAST JEDI (2017) | Full Movie Trailer | Full HD | 1080p</t>
+  </si>
+  <si>
+    <t>/watch?v=_iDA4_-TESM</t>
+  </si>
+  <si>
+    <t>READY PLAYER ONE - Official Trailer 1 [HD]</t>
+  </si>
+  <si>
+    <t>/watch?v=cSp1dM2Vj48&amp;t=51s</t>
+  </si>
+  <si>
+    <t>READY PLAYER ONE Final Trailer (2018)</t>
+  </si>
+  <si>
+    <t>/watch?v=ixWL1BWi44U&amp;t=172s</t>
+  </si>
+  <si>
+    <t>Ready Player One Comic-Con Trailer (2018) | Movieclips Trailers</t>
+  </si>
+  <si>
+    <t>/watch?v=LiK2fhOY0nE</t>
+  </si>
+  <si>
+    <t>Incredibles 2 Official Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=i5qOzqD9Rms&amp;t=36s</t>
+  </si>
+  <si>
+    <t>INCREDIBLES 2 Official Trailer #2 (2018) Disney Animated Superhero Movie HD</t>
+  </si>
+  <si>
+    <t>/watch?v=JwwY8gx_2LA</t>
+  </si>
+  <si>
+    <t>Incredibles 2 Official Teaser Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=ZJDMWVZta3M</t>
+  </si>
+  <si>
+    <t>Marvel Studios' Avengers: Infinity War Official Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=6ZfuNTqbHE8</t>
+  </si>
+  <si>
+    <t>Marvel Studios' Avengers: Infinity War - Official Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=QwievZ1Tx-8</t>
+  </si>
+  <si>
+    <t>AVENGERS INFINITY WAR Official Trailer 3 - 1 (Extended) Marvel</t>
+  </si>
+  <si>
+    <t>/watch?v=mdRo6HIaWEc</t>
+  </si>
+  <si>
+    <t>The LEGO Batman Movie Official Comic-Con Trailer (2017) - Will Arnett Movie</t>
+  </si>
+  <si>
+    <t>/watch?v=h6DOpfJzmo0</t>
+  </si>
+  <si>
+    <t>THE LEGO BATMAN MOVIE Trailer 1 - 3 (2017)</t>
+  </si>
+  <si>
+    <t>/watch?v=LZSQTVdF3QM</t>
+  </si>
+  <si>
+    <t>The Lego Batman Movie Official Trailer 4 (2017) - Will Arnett Movie</t>
+  </si>
+  <si>
+    <t>/watch?v=LqrQKZlCcjo</t>
+  </si>
+  <si>
+    <t>The Boss Baby Official Trailer #1 (2017) Alec Baldwin, Lisa Kudrow Animated Movie HD</t>
+  </si>
+  <si>
+    <t>/watch?v=r8kE7rSzfQs&amp;t=1s</t>
+  </si>
+  <si>
+    <t>The Boss Baby Official Trailer 1 (2017) - Alec Baldwin Movie</t>
+  </si>
+  <si>
+    <t>/watch?v=k397HRbTtWI</t>
+  </si>
+  <si>
+    <t>THE BOSS BABY | Official Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=Ud8j5GaqH3c</t>
+  </si>
+  <si>
+    <t>Inside Out - Official US Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=yRUAzGQ3nSY</t>
+  </si>
+  <si>
+    <t>Inside Out Official Trailer #2 (2015) - Disney Pixar Movie HD</t>
+  </si>
+  <si>
+    <t>/watch?v=seMwpP0yeu4</t>
+  </si>
+  <si>
+    <t>Inside Out 2 - 2020 Movie Trailer</t>
+  </si>
+  <si>
+    <t>/watch?v=3bjHLsZWHgg</t>
   </si>
 </sst>
 </file>
@@ -381,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BF02A3-3282-414E-ABDD-8E45600DA7E8}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -400,10 +565,22 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -412,7 +589,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -421,7 +604,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -430,7 +619,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -439,7 +634,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -448,27 +649,244 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"fixing it up for orchestrator"
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine.Moore\Documents\UiPath\HUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A8AF04-E49A-476B-8E1D-60406DF81975}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B90724-4DC9-4EC6-83CB-5ECFB8E5F1D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="570" yWindow="570" windowWidth="9600" windowHeight="4965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="83">
   <si>
     <t>Movie Name</t>
   </si>
@@ -231,22 +231,52 @@
     <t>Interstellar</t>
   </si>
   <si>
-    <t>Interstellar - Trailer - Official Warner Bros. UK</t>
-  </si>
-  <si>
-    <t>/watch?v=zSWdZVtXT7E&amp;t=20s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warner Bros. UK  </t>
-  </si>
-  <si>
-    <t>Published on May 16, 2014</t>
-  </si>
-  <si>
     <t xml:space="preserve">Warner Bros. Pictures  </t>
   </si>
   <si>
     <t>Published on Jul 27, 2017</t>
+  </si>
+  <si>
+    <t>/watch?v=xjDjIWPwcPU&amp;t=51s</t>
+  </si>
+  <si>
+    <t>/watch?v=dxWvtMOGAhw&amp;t=7s</t>
+  </si>
+  <si>
+    <t>/watch?v=yLNLPECROMA&amp;t=4s</t>
+  </si>
+  <si>
+    <t>IT CHAPTER TWO - Final Trailer [HD]</t>
+  </si>
+  <si>
+    <t>/watch?v=xhJ5P7Up3jA&amp;t=11s</t>
+  </si>
+  <si>
+    <t>Published on Jul 18, 2019</t>
+  </si>
+  <si>
+    <t>Published on Mar 29, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star Wars  </t>
+  </si>
+  <si>
+    <t>Published on Oct 9, 2017</t>
+  </si>
+  <si>
+    <t>Views</t>
+  </si>
+  <si>
+    <t>Likes</t>
+  </si>
+  <si>
+    <t>Dislikes</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Published Date</t>
   </si>
 </sst>
 </file>
@@ -262,12 +292,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -282,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -290,6 +326,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +664,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -920,41 +957,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8240E542-3620-4AB2-AF89-A9940611ABD7}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" customWidth="1"/>
     <col min="4" max="4" width="27.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1">
-        <v>27517906</v>
-      </c>
-      <c r="E1" s="1">
-        <v>90529</v>
-      </c>
-      <c r="F1" s="1">
-        <v>3580</v>
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="H1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -977,10 +1021,88 @@
         <v>14287</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1">
+        <v>18751440</v>
+      </c>
+      <c r="E3" s="1">
+        <v>326732</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6855</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>54958825</v>
+      </c>
+      <c r="E4" s="1">
+        <v>487087</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25857</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1">
+        <v>53281629</v>
+      </c>
+      <c r="E5" s="1">
+        <v>764396</v>
+      </c>
+      <c r="F5" s="1">
+        <v>39440</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -990,7 +1112,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BAE3971-80BB-4C46-BDEB-9FA9C8460CCB}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A11"/>
@@ -1048,6 +1170,56 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1055,13 +1227,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E7C7D3-C3E2-429F-9031-2F802AB73538}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1076,35 +1251,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>